<commit_message>
Uppdaterat mätvärdet i Deca/Ellinor
</commit_message>
<xml_diff>
--- a/Decathlon.xlsx
+++ b/Decathlon.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -29,22 +29,37 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Hep 800M</t>
-  </si>
-  <si>
-    <t>Hej hejsson</t>
-  </si>
-  <si>
-    <t>Hep 200M</t>
-  </si>
-  <si>
-    <t>hej hejsson</t>
-  </si>
-  <si>
-    <t>Hep Javelin Throw</t>
-  </si>
-  <si>
-    <t>rune hej</t>
+    <t>Deca 100M</t>
+  </si>
+  <si>
+    <t>hej</t>
+  </si>
+  <si>
+    <t>Deca 400M</t>
+  </si>
+  <si>
+    <t>Deca 110M Hurdles</t>
+  </si>
+  <si>
+    <t>Deca 1500M</t>
+  </si>
+  <si>
+    <t>Deca Long Jump</t>
+  </si>
+  <si>
+    <t>Dec High Jump</t>
+  </si>
+  <si>
+    <t>Dec Pole Vault</t>
+  </si>
+  <si>
+    <t>Dec Discus Throw</t>
+  </si>
+  <si>
+    <t>Deca Javelin Throw</t>
+  </si>
+  <si>
+    <t>Deca Shot Put</t>
   </si>
 </sst>
 </file>
@@ -89,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -114,7 +129,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -123,44 +138,197 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>80.0</v>
+        <v>8.0</v>
       </c>
       <c r="E2" t="n">
-        <v>1824.0</v>
+        <v>1642.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>15.0</v>
+        <v>43.0</v>
       </c>
       <c r="E3" t="n">
-        <v>2010.0</v>
+        <v>1166.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1108.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1249.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n">
+        <v>305.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>531.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>375.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>531.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>245.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>531.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>7.0</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="n">
-        <v>70.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2010.0</v>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>620.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>531.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>531.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>531.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>531.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>531.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ändrat i text samt max och min på alla grenar. Max och min strax under eller strax över nu gällande världsrekord.
</commit_message>
<xml_diff>
--- a/Decathlon.xlsx
+++ b/Decathlon.xlsx
@@ -29,10 +29,10 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Hep 800M</t>
+    <t>Deca 1500M</t>
   </si>
   <si>
-    <t>hej</t>
+    <t>Linus</t>
   </si>
 </sst>
 </file>
@@ -102,7 +102,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -111,10 +111,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>70.0</v>
+        <v>400.0</v>
       </c>
       <c r="E2" t="n">
-        <v>2026.0</v>
+        <v>124.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uppdaterat med val av deltagare samt total poäng.
</commit_message>
<xml_diff>
--- a/Decathlon.xlsx
+++ b/Decathlon.xlsx
@@ -14,13 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
-    <t>ID</t>
+    <t>NAME</t>
   </si>
   <si>
     <t>Dec/Hep</t>
-  </si>
-  <si>
-    <t>NAME</t>
   </si>
   <si>
     <t>Result</t>
@@ -29,16 +26,19 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Hep 800M</t>
+    <t>Total</t>
   </si>
   <si>
-    <t>hej hejsson</t>
+    <t>sten</t>
   </si>
   <si>
-    <t>Hep Shot Put</t>
+    <t>Hep 200M</t>
   </si>
   <si>
-    <t>hej hopp</t>
+    <t>Flisa</t>
+  </si>
+  <si>
+    <t>Hep 800M</t>
   </si>
 </sst>
 </file>
@@ -107,54 +107,54 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2.0</v>
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="n">
+        <v>22.0</v>
+      </c>
       <c r="D2" t="n">
-        <v>150.0</v>
+        <v>1181.0</v>
       </c>
       <c r="E2" t="n">
-        <v>693.0</v>
+        <v>1181.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>6.0</v>
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
         <v>6</v>
       </c>
+      <c r="C3" t="n">
+        <v>25.0</v>
+      </c>
       <c r="D3" t="n">
-        <v>29.0</v>
+        <v>887.0</v>
       </c>
       <c r="E3" t="n">
-        <v>693.0</v>
+        <v>887.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2.0</v>
+      <c r="A4" t="s">
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="n">
+        <v>98.0</v>
+      </c>
       <c r="D4" t="n">
-        <v>89.0</v>
+        <v>1486.0</v>
       </c>
       <c r="E4" t="n">
-        <v>1651.0</v>
+        <v>2667.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slagit isär totalpoängen för Deca och Hep i GUI
</commit_message>
<xml_diff>
--- a/Decathlon.xlsx
+++ b/Decathlon.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>NAME</t>
   </si>
@@ -29,16 +29,13 @@
     <t>Total</t>
   </si>
   <si>
-    <t>sten</t>
+    <t>Erik</t>
   </si>
   <si>
     <t>Hep 200M</t>
   </si>
   <si>
-    <t>Flisa</t>
-  </si>
-  <si>
-    <t>Hep 800M</t>
+    <t>Linus</t>
   </si>
 </sst>
 </file>
@@ -83,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -114,13 +111,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>22.0</v>
+        <v>20.0</v>
       </c>
       <c r="D2" t="n">
-        <v>1181.0</v>
+        <v>1398.0</v>
       </c>
       <c r="E2" t="n">
-        <v>1181.0</v>
+        <v>1398.0</v>
       </c>
     </row>
     <row r="3">
@@ -131,30 +128,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>25.0</v>
+        <v>19.0</v>
       </c>
       <c r="D3" t="n">
-        <v>887.0</v>
+        <v>1512.0</v>
       </c>
       <c r="E3" t="n">
-        <v>887.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
-        <v>98.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1486.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2667.0</v>
+        <v>1512.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>